<commit_message>
crash-analysis complete /w crypto variant
</commit_message>
<xml_diff>
--- a/outputs/per_event_metrics.xlsx
+++ b/outputs/per_event_metrics.xlsx
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.1278316965386729</v>
+        <v>-0.1278310765944046</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2898052867561227</v>
+        <v>0.2898055403637234</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2018301466072955</v>
+        <v>-0.201830196463171</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.2018301466072955</v>
+        <v>-0.201830196463171</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" s="2" t="n">
@@ -535,16 +535,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.3265014248494242</v>
+        <v>-0.326501396087418</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4959603835527287</v>
+        <v>0.4959609076700841</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.3371727505299607</v>
+        <v>-0.3371728154001947</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3371727505299607</v>
+        <v>-0.3371728154001947</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" s="2" t="n">
@@ -569,16 +569,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.2057346929729378</v>
+        <v>-0.2057347477567026</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1321672217017108</v>
+        <v>0.1321671306093944</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2111515184484098</v>
+        <v>-0.2111515974088592</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2111515184484098</v>
+        <v>-0.2111515974088592</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" s="2" t="n">
@@ -603,16 +603,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.2097997597095738</v>
+        <v>-0.2097999022555614</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2027348992047054</v>
+        <v>0.202735104988125</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2449638130506699</v>
+        <v>-0.2449638130506701</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2449638130506699</v>
+        <v>-0.2449638130506701</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="2" t="n">
@@ -637,16 +637,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.009236020702812486</v>
+        <v>-0.00923555994851577</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1771197340222497</v>
+        <v>0.1771198820623565</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.07813551874592728</v>
+        <v>-0.07813570574418682</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.07813551874592728</v>
+        <v>-0.07813570574418682</v>
       </c>
       <c r="G6" t="n">
         <v>24</v>
@@ -673,16 +673,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.0340390590458064</v>
+        <v>-0.03403942326633425</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3208156939228823</v>
+        <v>0.3208160723244858</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1419571930581572</v>
+        <v>-0.1419572801781036</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1419571930581572</v>
+        <v>-0.1419572801781036</v>
       </c>
       <c r="G7" t="n">
         <v>24</v>

</xml_diff>